<commit_message>
Co sua giao dien
</commit_message>
<xml_diff>
--- a/upload/KE HOACH GIANG DAY HTTT K42.xlsx
+++ b/upload/KE HOACH GIANG DAY HTTT K42.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="195" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="105">
   <si>
     <t>TRƯỜNG CAO ĐẲNG CẦN THƠ</t>
   </si>
@@ -322,15 +322,6 @@
     </r>
   </si>
   <si>
-    <t>PCCM</t>
-  </si>
-  <si>
-    <t>LT</t>
-  </si>
-  <si>
-    <t>TH</t>
-  </si>
-  <si>
     <t>Cần Thơ, ngày 21 tháng 12 năm 2017</t>
   </si>
   <si>
@@ -386,13 +377,13 @@
     </r>
   </si>
   <si>
-    <t>Ngành đào tạo: Quản trị mạng    Mã ngành: 6480209</t>
-  </si>
-  <si>
     <t>AC010</t>
   </si>
   <si>
     <t>AC070</t>
+  </si>
+  <si>
+    <t>Ngành đào tạo: Hệ thống thông tin    Mã ngành: 6320201</t>
   </si>
 </sst>
 </file>
@@ -566,8 +557,14 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -593,14 +590,8 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1001,8 +992,8 @@
   </sheetPr>
   <dimension ref="A1:L78"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A36" workbookViewId="0">
-      <selection activeCell="B28" sqref="B28"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6:J6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1018,96 +1009,94 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A1" s="27" t="s">
+      <c r="A1" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="27"/>
-      <c r="C1" s="27"/>
-      <c r="E1" s="17" t="s">
+      <c r="B1" s="18"/>
+      <c r="C1" s="18"/>
+      <c r="E1" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="F1" s="17"/>
-      <c r="G1" s="17"/>
-      <c r="H1" s="17"/>
-      <c r="I1" s="17"/>
-      <c r="J1" s="17"/>
+      <c r="F1" s="19"/>
+      <c r="G1" s="19"/>
+      <c r="H1" s="19"/>
+      <c r="I1" s="19"/>
+      <c r="J1" s="19"/>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A2" s="17" t="s">
+      <c r="A2" s="19" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="17"/>
-      <c r="C2" s="17"/>
-      <c r="E2" s="17" t="s">
-        <v>3</v>
-      </c>
-      <c r="F2" s="17"/>
-      <c r="G2" s="17"/>
-      <c r="H2" s="17"/>
-      <c r="I2" s="17"/>
-      <c r="J2" s="17"/>
+      <c r="B2" s="19"/>
+      <c r="C2" s="19"/>
+      <c r="E2" s="19" t="s">
+        <v>3</v>
+      </c>
+      <c r="F2" s="19"/>
+      <c r="G2" s="19"/>
+      <c r="H2" s="19"/>
+      <c r="I2" s="19"/>
+      <c r="J2" s="19"/>
     </row>
     <row r="4" spans="1:12" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A4" s="26" t="s">
+      <c r="A4" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="26"/>
-      <c r="C4" s="26"/>
-      <c r="D4" s="26"/>
-      <c r="E4" s="26"/>
-      <c r="F4" s="26"/>
-      <c r="G4" s="26"/>
-      <c r="H4" s="26"/>
-      <c r="I4" s="26"/>
-      <c r="J4" s="26"/>
+      <c r="B4" s="17"/>
+      <c r="C4" s="17"/>
+      <c r="D4" s="17"/>
+      <c r="E4" s="17"/>
+      <c r="F4" s="17"/>
+      <c r="G4" s="17"/>
+      <c r="H4" s="17"/>
+      <c r="I4" s="17"/>
+      <c r="J4" s="17"/>
     </row>
     <row r="5" spans="1:12" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="26" t="s">
-        <v>105</v>
-      </c>
-      <c r="B5" s="26"/>
-      <c r="C5" s="26"/>
-      <c r="D5" s="26"/>
-      <c r="E5" s="26"/>
-      <c r="F5" s="26"/>
-      <c r="G5" s="26"/>
-      <c r="H5" s="26"/>
-      <c r="I5" s="26"/>
-      <c r="J5" s="26"/>
+      <c r="A5" s="17" t="s">
+        <v>104</v>
+      </c>
+      <c r="B5" s="17"/>
+      <c r="C5" s="17"/>
+      <c r="D5" s="17"/>
+      <c r="E5" s="17"/>
+      <c r="F5" s="17"/>
+      <c r="G5" s="17"/>
+      <c r="H5" s="17"/>
+      <c r="I5" s="17"/>
+      <c r="J5" s="17"/>
     </row>
     <row r="6" spans="1:12" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="19" t="s">
+      <c r="A6" s="21" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="19"/>
-      <c r="C6" s="19"/>
-      <c r="D6" s="19"/>
-      <c r="E6" s="19"/>
-      <c r="F6" s="19"/>
-      <c r="G6" s="19"/>
-      <c r="H6" s="19"/>
-      <c r="I6" s="19"/>
-      <c r="J6" s="19"/>
+      <c r="B6" s="21"/>
+      <c r="C6" s="21"/>
+      <c r="D6" s="21"/>
+      <c r="E6" s="21"/>
+      <c r="F6" s="21"/>
+      <c r="G6" s="21"/>
+      <c r="H6" s="21"/>
+      <c r="I6" s="21"/>
+      <c r="J6" s="21"/>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A8" s="20" t="s">
-        <v>101</v>
-      </c>
-      <c r="B8" s="20"/>
-      <c r="C8" s="20"/>
-      <c r="D8" s="20"/>
-      <c r="E8" s="20"/>
-      <c r="F8" s="20"/>
-      <c r="G8" s="20"/>
-      <c r="H8" s="20"/>
-      <c r="I8" s="20"/>
-      <c r="J8" s="20"/>
+      <c r="A8" s="22" t="s">
+        <v>98</v>
+      </c>
+      <c r="B8" s="22"/>
+      <c r="C8" s="22"/>
+      <c r="D8" s="22"/>
+      <c r="E8" s="22"/>
+      <c r="F8" s="22"/>
+      <c r="G8" s="22"/>
+      <c r="H8" s="22"/>
+      <c r="I8" s="22"/>
+      <c r="J8" s="22"/>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="K9" s="25" t="s">
-        <v>97</v>
-      </c>
-      <c r="L9" s="25"/>
+      <c r="K9" s="16"/>
+      <c r="L9" s="16"/>
     </row>
     <row r="10" spans="1:12" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
@@ -1140,12 +1129,6 @@
       <c r="J10" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="K10" s="2" t="s">
-        <v>98</v>
-      </c>
-      <c r="L10" s="2" t="s">
-        <v>99</v>
-      </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" s="6">
@@ -1174,10 +1157,6 @@
       <c r="J11" s="6">
         <v>3</v>
       </c>
-      <c r="L11" s="2">
-        <f>D11+D12+D13+D14+D15+D24+D25+D26+D27+D16</f>
-        <v>3</v>
-      </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" s="6">
@@ -1268,7 +1247,7 @@
         <v>5</v>
       </c>
       <c r="B15" s="10" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="C15" s="8" t="s">
         <v>94</v>
@@ -1320,14 +1299,8 @@
       <c r="J16" s="6">
         <v>4</v>
       </c>
-      <c r="K16" s="2">
-        <v>30</v>
-      </c>
-      <c r="L16" s="2">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="17" spans="1:12" ht="31.5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="17" spans="1:10" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A17" s="6">
         <v>7</v>
       </c>
@@ -1356,14 +1329,8 @@
       <c r="J17" s="6">
         <v>3</v>
       </c>
-      <c r="K17" s="2">
-        <v>45</v>
-      </c>
-      <c r="L17" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" s="6">
         <v>8</v>
       </c>
@@ -1392,19 +1359,13 @@
       <c r="J18" s="6">
         <v>4</v>
       </c>
-      <c r="K18" s="2">
-        <v>45</v>
-      </c>
-      <c r="L18" s="2">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A19" s="21" t="s">
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A19" s="23" t="s">
         <v>31</v>
       </c>
-      <c r="B19" s="22"/>
-      <c r="C19" s="23"/>
+      <c r="B19" s="24"/>
+      <c r="C19" s="25"/>
       <c r="D19" s="11">
         <f>SUM(D11:D18)</f>
         <v>8</v>
@@ -1428,22 +1389,22 @@
         <v>25</v>
       </c>
     </row>
-    <row r="20" spans="1:12" ht="44.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A21" s="20" t="s">
-        <v>102</v>
-      </c>
-      <c r="B21" s="20"/>
-      <c r="C21" s="20"/>
-      <c r="D21" s="20"/>
-      <c r="E21" s="20"/>
-      <c r="F21" s="20"/>
-      <c r="G21" s="20"/>
-      <c r="H21" s="20"/>
-      <c r="I21" s="20"/>
-      <c r="J21" s="20"/>
-    </row>
-    <row r="23" spans="1:12" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:10" ht="44.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A21" s="22" t="s">
+        <v>99</v>
+      </c>
+      <c r="B21" s="22"/>
+      <c r="C21" s="22"/>
+      <c r="D21" s="22"/>
+      <c r="E21" s="22"/>
+      <c r="F21" s="22"/>
+      <c r="G21" s="22"/>
+      <c r="H21" s="22"/>
+      <c r="I21" s="22"/>
+      <c r="J21" s="22"/>
+    </row>
+    <row r="23" spans="1:10" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
         <v>6</v>
       </c>
@@ -1475,7 +1436,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24" s="6">
         <v>1</v>
       </c>
@@ -1503,7 +1464,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" s="6">
         <v>2</v>
       </c>
@@ -1531,7 +1492,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="26" spans="1:12" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:10" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A26" s="6">
         <v>3</v>
       </c>
@@ -1559,12 +1520,12 @@
         <v>2</v>
       </c>
     </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27" s="6">
         <v>4</v>
       </c>
       <c r="B27" s="10" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="C27" s="8" t="s">
         <v>95</v>
@@ -1587,7 +1548,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28" s="6">
         <v>5</v>
       </c>
@@ -1617,7 +1578,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29" s="6">
         <v>6</v>
       </c>
@@ -1646,14 +1607,8 @@
       <c r="J29" s="6">
         <v>4</v>
       </c>
-      <c r="K29" s="2">
-        <v>45</v>
-      </c>
-      <c r="L29" s="2">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A30" s="6">
         <v>7</v>
       </c>
@@ -1682,14 +1637,8 @@
       <c r="J30" s="6">
         <v>4</v>
       </c>
-      <c r="K30" s="2">
-        <v>45</v>
-      </c>
-      <c r="L30" s="2">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A31" s="6">
         <v>8</v>
       </c>
@@ -1718,14 +1667,8 @@
       <c r="J31" s="6">
         <v>4</v>
       </c>
-      <c r="K31" s="2">
-        <v>60</v>
-      </c>
-      <c r="L31" s="2">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A32" s="6">
         <v>9</v>
       </c>
@@ -1754,11 +1697,11 @@
       </c>
     </row>
     <row r="33" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A33" s="18" t="s">
+      <c r="A33" s="20" t="s">
         <v>31</v>
       </c>
-      <c r="B33" s="18"/>
-      <c r="C33" s="18"/>
+      <c r="B33" s="20"/>
+      <c r="C33" s="20"/>
       <c r="D33" s="11">
         <f>SUM(D24:D32)</f>
         <v>11</v>
@@ -1784,18 +1727,18 @@
     </row>
     <row r="34" spans="1:10" ht="78.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="35" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A35" s="20" t="s">
-        <v>103</v>
-      </c>
-      <c r="B35" s="20"/>
-      <c r="C35" s="20"/>
-      <c r="D35" s="20"/>
-      <c r="E35" s="20"/>
-      <c r="F35" s="20"/>
-      <c r="G35" s="20"/>
-      <c r="H35" s="20"/>
-      <c r="I35" s="20"/>
-      <c r="J35" s="20"/>
+      <c r="A35" s="22" t="s">
+        <v>100</v>
+      </c>
+      <c r="B35" s="22"/>
+      <c r="C35" s="22"/>
+      <c r="D35" s="22"/>
+      <c r="E35" s="22"/>
+      <c r="F35" s="22"/>
+      <c r="G35" s="22"/>
+      <c r="H35" s="22"/>
+      <c r="I35" s="22"/>
+      <c r="J35" s="22"/>
     </row>
     <row r="37" spans="1:10" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A37" s="3" t="s">
@@ -2038,11 +1981,11 @@
       </c>
     </row>
     <row r="45" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A45" s="18" t="s">
+      <c r="A45" s="20" t="s">
         <v>31</v>
       </c>
-      <c r="B45" s="18"/>
-      <c r="C45" s="18"/>
+      <c r="B45" s="20"/>
+      <c r="C45" s="20"/>
       <c r="D45" s="11">
         <f>SUM(D38:D43)</f>
         <v>17</v>
@@ -2067,20 +2010,20 @@
       </c>
     </row>
     <row r="47" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A47" s="20" t="s">
+      <c r="A47" s="22" t="s">
         <v>96</v>
       </c>
-      <c r="B47" s="20"/>
-      <c r="C47" s="20"/>
-      <c r="D47" s="20"/>
-      <c r="E47" s="20"/>
-      <c r="F47" s="20"/>
-      <c r="G47" s="20"/>
-      <c r="H47" s="20"/>
-      <c r="I47" s="20"/>
-      <c r="J47" s="20"/>
-    </row>
-    <row r="49" spans="1:11" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="B47" s="22"/>
+      <c r="C47" s="22"/>
+      <c r="D47" s="22"/>
+      <c r="E47" s="22"/>
+      <c r="F47" s="22"/>
+      <c r="G47" s="22"/>
+      <c r="H47" s="22"/>
+      <c r="I47" s="22"/>
+      <c r="J47" s="22"/>
+    </row>
+    <row r="49" spans="1:10" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A49" s="3" t="s">
         <v>6</v>
       </c>
@@ -2112,7 +2055,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="50" spans="1:11" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:10" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="6">
         <v>1</v>
       </c>
@@ -2142,7 +2085,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="51" spans="1:11" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:10" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="6">
         <v>2</v>
       </c>
@@ -2172,7 +2115,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="52" spans="1:11" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:10" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52" s="6">
         <v>3</v>
       </c>
@@ -2202,7 +2145,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="53" spans="1:11" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:10" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A53" s="6">
         <v>4</v>
       </c>
@@ -2232,7 +2175,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="54" spans="1:11" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:10" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A54" s="6">
         <v>5</v>
       </c>
@@ -2262,7 +2205,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="55" spans="1:11" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:10" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A55" s="6">
         <v>6</v>
       </c>
@@ -2292,7 +2235,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="1:11" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:10" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A56" s="6">
         <v>7</v>
       </c>
@@ -2320,12 +2263,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A57" s="18" t="s">
+    <row r="57" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A57" s="20" t="s">
         <v>31</v>
       </c>
-      <c r="B57" s="18"/>
-      <c r="C57" s="18"/>
+      <c r="B57" s="20"/>
+      <c r="C57" s="20"/>
       <c r="D57" s="11">
         <f>SUM(D50:D56)</f>
         <v>16</v>
@@ -2349,21 +2292,21 @@
         <v>20</v>
       </c>
     </row>
-    <row r="59" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A59" s="20" t="s">
-        <v>104</v>
-      </c>
-      <c r="B59" s="20"/>
-      <c r="C59" s="20"/>
-      <c r="D59" s="20"/>
-      <c r="E59" s="20"/>
-      <c r="F59" s="20"/>
-      <c r="G59" s="20"/>
-      <c r="H59" s="20"/>
-      <c r="I59" s="20"/>
-      <c r="J59" s="20"/>
-    </row>
-    <row r="61" spans="1:11" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A59" s="22" t="s">
+        <v>101</v>
+      </c>
+      <c r="B59" s="22"/>
+      <c r="C59" s="22"/>
+      <c r="D59" s="22"/>
+      <c r="E59" s="22"/>
+      <c r="F59" s="22"/>
+      <c r="G59" s="22"/>
+      <c r="H59" s="22"/>
+      <c r="I59" s="22"/>
+      <c r="J59" s="22"/>
+    </row>
+    <row r="61" spans="1:10" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A61" s="3" t="s">
         <v>6</v>
       </c>
@@ -2395,7 +2338,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="62" spans="1:11" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:10" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A62" s="6">
         <v>1</v>
       </c>
@@ -2424,12 +2367,8 @@
       <c r="J62" s="6">
         <v>4</v>
       </c>
-      <c r="K62" s="2">
-        <f>SUM(D62:D64,D66,D67)+SUM(D50:D55)+SUM(D38:D43)+SUM(D29:D31)+SUM(D17:D18)</f>
-        <v>58</v>
-      </c>
-    </row>
-    <row r="63" spans="1:11" ht="47.25" x14ac:dyDescent="0.25">
+    </row>
+    <row r="63" spans="1:10" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A63" s="6">
         <v>2</v>
       </c>
@@ -2459,7 +2398,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="64" spans="1:11" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:10" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A64" s="6">
         <v>3</v>
       </c>
@@ -2548,7 +2487,7 @@
       </c>
     </row>
     <row r="67" spans="1:10" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A67" s="24">
+      <c r="A67" s="26">
         <v>6</v>
       </c>
       <c r="B67" s="9" t="s">
@@ -2578,7 +2517,7 @@
       </c>
     </row>
     <row r="68" spans="1:10" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A68" s="24"/>
+      <c r="A68" s="26"/>
       <c r="B68" s="9" t="s">
         <v>85</v>
       </c>
@@ -2606,7 +2545,7 @@
       </c>
     </row>
     <row r="69" spans="1:10" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A69" s="24"/>
+      <c r="A69" s="26"/>
       <c r="B69" s="9" t="s">
         <v>87</v>
       </c>
@@ -2634,7 +2573,7 @@
       </c>
     </row>
     <row r="70" spans="1:10" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A70" s="24"/>
+      <c r="A70" s="26"/>
       <c r="B70" s="9" t="s">
         <v>89</v>
       </c>
@@ -2662,11 +2601,11 @@
       </c>
     </row>
     <row r="71" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A71" s="18" t="s">
+      <c r="A71" s="20" t="s">
         <v>31</v>
       </c>
-      <c r="B71" s="18"/>
-      <c r="C71" s="18"/>
+      <c r="B71" s="20"/>
+      <c r="C71" s="20"/>
       <c r="D71" s="11">
         <f>SUM(D62:D67)</f>
         <v>11</v>
@@ -2691,48 +2630,46 @@
       </c>
     </row>
     <row r="73" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="G73" s="16" t="s">
-        <v>100</v>
-      </c>
-      <c r="H73" s="16"/>
-      <c r="I73" s="16"/>
-      <c r="J73" s="16"/>
+      <c r="G73" s="27" t="s">
+        <v>97</v>
+      </c>
+      <c r="H73" s="27"/>
+      <c r="I73" s="27"/>
+      <c r="J73" s="27"/>
     </row>
     <row r="74" spans="1:10" s="15" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A74" s="17" t="s">
+      <c r="A74" s="19" t="s">
         <v>91</v>
       </c>
-      <c r="B74" s="17"/>
-      <c r="C74" s="17"/>
-      <c r="D74" s="17" t="s">
+      <c r="B74" s="19"/>
+      <c r="C74" s="19"/>
+      <c r="D74" s="19" t="s">
         <v>92</v>
       </c>
-      <c r="E74" s="17"/>
-      <c r="F74" s="17"/>
-      <c r="G74" s="17" t="s">
+      <c r="E74" s="19"/>
+      <c r="F74" s="19"/>
+      <c r="G74" s="19" t="s">
         <v>2</v>
       </c>
-      <c r="H74" s="17"/>
-      <c r="I74" s="17"/>
-      <c r="J74" s="17"/>
+      <c r="H74" s="19"/>
+      <c r="I74" s="19"/>
+      <c r="J74" s="19"/>
     </row>
     <row r="77" spans="1:10" ht="37.5" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="78" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A78" s="17" t="s">
+      <c r="A78" s="19" t="s">
         <v>93</v>
       </c>
-      <c r="B78" s="17"/>
-      <c r="C78" s="17"/>
+      <c r="B78" s="19"/>
+      <c r="C78" s="19"/>
     </row>
   </sheetData>
   <mergeCells count="24">
-    <mergeCell ref="K9:L9"/>
-    <mergeCell ref="A5:J5"/>
-    <mergeCell ref="A1:C1"/>
-    <mergeCell ref="E1:J1"/>
-    <mergeCell ref="A2:C2"/>
-    <mergeCell ref="E2:J2"/>
-    <mergeCell ref="A4:J4"/>
+    <mergeCell ref="G73:J73"/>
+    <mergeCell ref="A74:C74"/>
+    <mergeCell ref="D74:F74"/>
+    <mergeCell ref="G74:J74"/>
+    <mergeCell ref="A78:C78"/>
     <mergeCell ref="A71:C71"/>
     <mergeCell ref="A6:J6"/>
     <mergeCell ref="A8:J8"/>
@@ -2745,11 +2682,13 @@
     <mergeCell ref="A57:C57"/>
     <mergeCell ref="A59:J59"/>
     <mergeCell ref="A67:A70"/>
-    <mergeCell ref="G73:J73"/>
-    <mergeCell ref="A74:C74"/>
-    <mergeCell ref="D74:F74"/>
-    <mergeCell ref="G74:J74"/>
-    <mergeCell ref="A78:C78"/>
+    <mergeCell ref="K9:L9"/>
+    <mergeCell ref="A5:J5"/>
+    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="E1:J1"/>
+    <mergeCell ref="A2:C2"/>
+    <mergeCell ref="E2:J2"/>
+    <mergeCell ref="A4:J4"/>
   </mergeCells>
   <pageMargins left="0.2" right="0.2" top="0.5" bottom="0.5" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="97" fitToHeight="0" orientation="portrait" verticalDpi="0" r:id="rId1"/>

</xml_diff>